<commit_message>
Son teslim tarihi ve veri güncellemeleri
</commit_message>
<xml_diff>
--- a/mail_merge_wide_3kalem.xlsx
+++ b/mail_merge_wide_3kalem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trakyaedutr-my.sharepoint.com/personal/oirmakcetin_trakya_edu_tr/Documents/Documents/Olgun/Lisans/Gümrük İşletme Bölümü/Bilge Dersi/Bilge 1/Bilge_1_Son3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{B398E1CC-67E7-4AB0-99E6-2A6A63733B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B26D4F7B-5340-4030-84ED-B14A9E2A2E30}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{B398E1CC-67E7-4AB0-99E6-2A6A63733B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2F1C326-BFFB-4038-A954-A672326FDFC2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2208,7 +2208,7 @@
     <col min="93" max="93" width="23.36328125" customWidth="1"/>
     <col min="94" max="94" width="11.81640625" customWidth="1"/>
     <col min="95" max="95" width="8.7265625" customWidth="1"/>
-    <col min="96" max="96" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:97" x14ac:dyDescent="0.35">
@@ -2807,12 +2807,15 @@
       </c>
       <c r="CP2">
         <f t="shared" ref="CP2:CP33" ca="1" si="14">RAND()</f>
-        <v>0.12860021876190719</v>
+        <v>0.73749831401699018</v>
       </c>
       <c r="CQ2">
         <v>1</v>
       </c>
-      <c r="CR2" s="10"/>
+      <c r="CR2" s="10" t="str">
+        <f>"20.12.2025 22:00"</f>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -3119,10 +3122,14 @@
       </c>
       <c r="CP3">
         <f t="shared" ca="1" si="14"/>
-        <v>0.78715979094807698</v>
+        <v>0.40970069810620524</v>
       </c>
       <c r="CQ3">
         <v>1</v>
+      </c>
+      <c r="CR3" s="10" t="str">
+        <f t="shared" ref="CR3:CR57" si="15">"20.12.2025 22:00"</f>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.35">
@@ -3426,10 +3433,14 @@
       </c>
       <c r="CP4">
         <f t="shared" ca="1" si="14"/>
-        <v>0.63414248113145999</v>
+        <v>2.2282645245251587E-2</v>
       </c>
       <c r="CQ4">
         <v>1</v>
+      </c>
+      <c r="CR4" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="5" spans="1:97" x14ac:dyDescent="0.35">
@@ -3736,10 +3747,14 @@
       </c>
       <c r="CP5">
         <f t="shared" ca="1" si="14"/>
-        <v>3.9243509685032318E-2</v>
+        <v>0.94162203197954841</v>
       </c>
       <c r="CQ5">
         <v>1</v>
+      </c>
+      <c r="CR5" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="6" spans="1:97" x14ac:dyDescent="0.35">
@@ -4046,10 +4061,14 @@
       </c>
       <c r="CP6">
         <f t="shared" ca="1" si="14"/>
-        <v>0.59688263582203005</v>
+        <v>0.75154897569586265</v>
       </c>
       <c r="CQ6">
         <v>1</v>
+      </c>
+      <c r="CR6" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="7" spans="1:97" x14ac:dyDescent="0.35">
@@ -4357,10 +4376,14 @@
       </c>
       <c r="CP7">
         <f t="shared" ca="1" si="14"/>
-        <v>0.13966791317266247</v>
+        <v>0.99805332284840087</v>
       </c>
       <c r="CQ7">
         <v>1</v>
+      </c>
+      <c r="CR7" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="8" spans="1:97" x14ac:dyDescent="0.35">
@@ -4667,10 +4690,14 @@
       </c>
       <c r="CP8">
         <f t="shared" ca="1" si="14"/>
-        <v>0.96004688825567774</v>
+        <v>0.58553741273059534</v>
       </c>
       <c r="CQ8">
         <v>1</v>
+      </c>
+      <c r="CR8" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="9" spans="1:97" x14ac:dyDescent="0.35">
@@ -4822,11 +4849,11 @@
         <v>522.11424</v>
       </c>
       <c r="AV9" s="6">
-        <f t="shared" ref="AV9:AV32" si="15">AU9-AQ9</f>
+        <f t="shared" ref="AV9:AV32" si="16">AU9-AQ9</f>
         <v>87.019039999999961</v>
       </c>
       <c r="AW9" s="6">
-        <f t="shared" ref="AW9:AW32" si="16">AU9</f>
+        <f t="shared" ref="AW9:AW32" si="17">AU9</f>
         <v>522.11424</v>
       </c>
       <c r="AX9" t="s">
@@ -4977,10 +5004,14 @@
       </c>
       <c r="CP9">
         <f t="shared" ca="1" si="14"/>
-        <v>0.71101966045339848</v>
+        <v>0.42632560240779172</v>
       </c>
       <c r="CQ9">
         <v>1</v>
+      </c>
+      <c r="CR9" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="10" spans="1:97" x14ac:dyDescent="0.35">
@@ -5132,11 +5163,11 @@
         <v>1265.772438</v>
       </c>
       <c r="AV10" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>261.19113799999991</v>
       </c>
       <c r="AW10" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1265.772438</v>
       </c>
       <c r="AX10" t="s">
@@ -5286,10 +5317,14 @@
       </c>
       <c r="CP10">
         <f t="shared" ca="1" si="14"/>
-        <v>0.85742466311113774</v>
+        <v>0.94184375493468575</v>
       </c>
       <c r="CQ10">
         <v>1</v>
+      </c>
+      <c r="CR10" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="11" spans="1:97" x14ac:dyDescent="0.35">
@@ -5441,11 +5476,11 @@
         <v>1271.2906799999998</v>
       </c>
       <c r="AV11" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>211.88177999999994</v>
       </c>
       <c r="AW11" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1271.2906799999998</v>
       </c>
       <c r="AX11" t="s">
@@ -5596,10 +5631,14 @@
       </c>
       <c r="CP11">
         <f t="shared" ca="1" si="14"/>
-        <v>5.1260415851700492E-2</v>
+        <v>0.68762786248459296</v>
       </c>
       <c r="CQ11">
         <v>1</v>
+      </c>
+      <c r="CR11" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="12" spans="1:97" x14ac:dyDescent="0.35">
@@ -5750,11 +5789,11 @@
         <v>2463.6621599999994</v>
       </c>
       <c r="AV12" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>410.61035999999967</v>
       </c>
       <c r="AW12" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2463.6621599999994</v>
       </c>
       <c r="AX12" t="s">
@@ -5905,10 +5944,14 @@
       </c>
       <c r="CP12">
         <f t="shared" ca="1" si="14"/>
-        <v>0.32018783055812006</v>
+        <v>0.86506851193075474</v>
       </c>
       <c r="CQ12">
         <v>1</v>
+      </c>
+      <c r="CR12" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="13" spans="1:97" x14ac:dyDescent="0.35">
@@ -6059,11 +6102,11 @@
         <v>1425.0881999999999</v>
       </c>
       <c r="AV13" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>237.51469999999995</v>
       </c>
       <c r="AW13" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1425.0881999999999</v>
       </c>
       <c r="AX13" t="s">
@@ -6213,10 +6256,14 @@
       </c>
       <c r="CP13">
         <f t="shared" ca="1" si="14"/>
-        <v>0.76723295669080172</v>
+        <v>0.49331134135751964</v>
       </c>
       <c r="CQ13">
         <v>1</v>
+      </c>
+      <c r="CR13" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="14" spans="1:97" x14ac:dyDescent="0.35">
@@ -6368,11 +6415,11 @@
         <v>643.43556000000001</v>
       </c>
       <c r="AV14" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>107.23925999999994</v>
       </c>
       <c r="AW14" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>643.43556000000001</v>
       </c>
       <c r="AX14" t="s">
@@ -6523,10 +6570,14 @@
       </c>
       <c r="CP14">
         <f t="shared" ca="1" si="14"/>
-        <v>0.26153017194298001</v>
+        <v>0.35588295138900317</v>
       </c>
       <c r="CQ14">
         <v>1</v>
+      </c>
+      <c r="CR14" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="15" spans="1:97" x14ac:dyDescent="0.35">
@@ -6678,11 +6729,11 @@
         <v>1305.8415599999998</v>
       </c>
       <c r="AV15" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>217.6402599999999</v>
       </c>
       <c r="AW15" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1305.8415599999998</v>
       </c>
       <c r="AX15" t="s">
@@ -6833,10 +6884,14 @@
       </c>
       <c r="CP15">
         <f t="shared" ca="1" si="14"/>
-        <v>0.19374483645051388</v>
+        <v>0.8875223454688258</v>
       </c>
       <c r="CQ15">
         <v>1</v>
+      </c>
+      <c r="CR15" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="16" spans="1:97" x14ac:dyDescent="0.35">
@@ -6989,11 +7044,11 @@
         <v>19128.159071999999</v>
       </c>
       <c r="AV16" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10272.529871999999</v>
       </c>
       <c r="AW16" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>19128.159071999999</v>
       </c>
       <c r="AX16" t="s">
@@ -7144,13 +7199,17 @@
       </c>
       <c r="CP16">
         <f t="shared" ca="1" si="14"/>
-        <v>0.10859129952581226</v>
+        <v>0.33998833688902008</v>
       </c>
       <c r="CQ16">
         <v>1</v>
       </c>
+      <c r="CR16" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1222603019</v>
       </c>
@@ -7299,11 +7358,11 @@
         <v>877.04561280000019</v>
       </c>
       <c r="AV17" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>224.48191280000015</v>
       </c>
       <c r="AW17" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>877.04561280000019</v>
       </c>
       <c r="AX17" t="s">
@@ -7454,13 +7513,17 @@
       </c>
       <c r="CP17">
         <f t="shared" ca="1" si="14"/>
-        <v>0.91251509619653304</v>
+        <v>0.47931716667744984</v>
       </c>
       <c r="CQ17">
         <v>1</v>
       </c>
+      <c r="CR17" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="18" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1222603020</v>
       </c>
@@ -7609,11 +7672,11 @@
         <v>1431.2322360000001</v>
       </c>
       <c r="AV18" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>295.33363600000007</v>
       </c>
       <c r="AW18" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1431.2322360000001</v>
       </c>
       <c r="AX18" t="s">
@@ -7763,13 +7826,17 @@
       </c>
       <c r="CP18">
         <f t="shared" ca="1" si="14"/>
-        <v>0.44430209577762869</v>
+        <v>0.10147490767344447</v>
       </c>
       <c r="CQ18">
         <v>1</v>
       </c>
+      <c r="CR18" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1222603022</v>
       </c>
@@ -7918,11 +7985,11 @@
         <v>462.9817920000001</v>
       </c>
       <c r="AV19" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>118.50129200000003</v>
       </c>
       <c r="AW19" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>462.9817920000001</v>
       </c>
       <c r="AX19" t="s">
@@ -8073,13 +8140,17 @@
       </c>
       <c r="CP19">
         <f t="shared" ca="1" si="14"/>
-        <v>0.283131208971658</v>
+        <v>0.73646537482766083</v>
       </c>
       <c r="CQ19">
         <v>1</v>
       </c>
+      <c r="CR19" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1222603023</v>
       </c>
@@ -8229,11 +8300,11 @@
         <v>718.09637759999998</v>
       </c>
       <c r="AV20" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>183.79847760000007</v>
       </c>
       <c r="AW20" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>718.09637759999998</v>
       </c>
       <c r="AX20" t="s">
@@ -8386,13 +8457,17 @@
       </c>
       <c r="CP20">
         <f t="shared" ca="1" si="14"/>
-        <v>0.42402303418345155</v>
+        <v>0.17230035921926912</v>
       </c>
       <c r="CQ20">
         <v>1</v>
       </c>
+      <c r="CR20" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1222603024</v>
       </c>
@@ -8541,11 +8616,11 @@
         <v>1496.1019200000001</v>
       </c>
       <c r="AV21" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>249.35032000000001</v>
       </c>
       <c r="AW21" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1496.1019200000001</v>
       </c>
       <c r="AX21" t="s">
@@ -8697,13 +8772,17 @@
       </c>
       <c r="CP21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.83195017718105346</v>
+        <v>0.13712485257088747</v>
       </c>
       <c r="CQ21">
         <v>1</v>
       </c>
+      <c r="CR21" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1222603025</v>
       </c>
@@ -8853,11 +8932,11 @@
         <v>17655.673247999999</v>
       </c>
       <c r="AV22" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9481.7504479999989</v>
       </c>
       <c r="AW22" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>17655.673247999999</v>
       </c>
       <c r="AX22" t="s">
@@ -9008,13 +9087,17 @@
       </c>
       <c r="CP22">
         <f t="shared" ca="1" si="14"/>
-        <v>0.77564968772142395</v>
+        <v>0.88170803563347944</v>
       </c>
       <c r="CQ22">
         <v>1</v>
       </c>
+      <c r="CR22" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1222603028</v>
       </c>
@@ -9163,11 +9246,11 @@
         <v>1069.9924800000001</v>
       </c>
       <c r="AV23" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>178.33208000000002</v>
       </c>
       <c r="AW23" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1069.9924800000001</v>
       </c>
       <c r="AX23" t="s">
@@ -9318,13 +9401,17 @@
       </c>
       <c r="CP23">
         <f t="shared" ca="1" si="14"/>
-        <v>0.93876104861228027</v>
+        <v>0.95992789462601524</v>
       </c>
       <c r="CQ23">
         <v>1</v>
       </c>
+      <c r="CR23" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1222603029</v>
       </c>
@@ -9474,11 +9561,11 @@
         <v>20825.593905599999</v>
       </c>
       <c r="AV24" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>12060.6133056</v>
       </c>
       <c r="AW24" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>20825.593905599999</v>
       </c>
       <c r="AX24" t="s">
@@ -9629,13 +9716,17 @@
       </c>
       <c r="CP24">
         <f t="shared" ca="1" si="14"/>
-        <v>0.56786978668572397</v>
+        <v>0.35671346866215792</v>
       </c>
       <c r="CQ24">
         <v>1</v>
       </c>
+      <c r="CR24" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1222603030</v>
       </c>
@@ -9784,11 +9875,11 @@
         <v>893.04804000000001</v>
       </c>
       <c r="AV25" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>148.84133999999995</v>
       </c>
       <c r="AW25" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>893.04804000000001</v>
       </c>
       <c r="AX25" t="s">
@@ -9939,13 +10030,17 @@
       </c>
       <c r="CP25">
         <f t="shared" ca="1" si="14"/>
-        <v>0.6971279331107969</v>
+        <v>0.96161402794923845</v>
       </c>
       <c r="CQ25">
         <v>1</v>
       </c>
+      <c r="CR25" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="26" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1222603031</v>
       </c>
@@ -10095,11 +10190,11 @@
         <v>18363.720038400003</v>
       </c>
       <c r="AV26" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10634.881638400002</v>
       </c>
       <c r="AW26" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>18363.720038400003</v>
       </c>
       <c r="AX26" t="s">
@@ -10250,13 +10345,17 @@
       </c>
       <c r="CP26">
         <f t="shared" ca="1" si="14"/>
-        <v>0.81753731392971885</v>
+        <v>0.35327281942397271</v>
       </c>
       <c r="CQ26">
         <v>1</v>
       </c>
+      <c r="CR26" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="27" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1222603032</v>
       </c>
@@ -10405,11 +10504,11 @@
         <v>1180.3708799999999</v>
       </c>
       <c r="AV27" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>196.72847999999988</v>
       </c>
       <c r="AW27" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1180.3708799999999</v>
       </c>
       <c r="AX27" t="s">
@@ -10561,13 +10660,17 @@
       </c>
       <c r="CP27">
         <f t="shared" ca="1" si="14"/>
-        <v>6.8452917331825236E-2</v>
+        <v>0.53323231877321964</v>
       </c>
       <c r="CQ27">
         <v>1</v>
       </c>
+      <c r="CR27" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="28" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1222603033</v>
       </c>
@@ -10716,11 +10819,11 @@
         <v>878.33543999999995</v>
       </c>
       <c r="AV28" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>146.38923999999997</v>
       </c>
       <c r="AW28" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>878.33543999999995</v>
       </c>
       <c r="AX28" t="s">
@@ -10871,13 +10974,17 @@
       </c>
       <c r="CP28">
         <f t="shared" ca="1" si="14"/>
-        <v>0.99892955733342159</v>
+        <v>0.52098868327070447</v>
       </c>
       <c r="CQ28">
         <v>1</v>
       </c>
+      <c r="CR28" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="29" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1222603034</v>
       </c>
@@ -11026,11 +11133,11 @@
         <v>2473.3711200000002</v>
       </c>
       <c r="AV29" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>412.22852000000012</v>
       </c>
       <c r="AW29" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2473.3711200000002</v>
       </c>
       <c r="AX29" t="s">
@@ -11182,13 +11289,17 @@
       </c>
       <c r="CP29">
         <f t="shared" ca="1" si="14"/>
-        <v>0.72700449604842232</v>
+        <v>0.32259151098561267</v>
       </c>
       <c r="CQ29">
         <v>1</v>
       </c>
+      <c r="CR29" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1222603035</v>
       </c>
@@ -11338,11 +11449,11 @@
         <v>1415.6273879999999</v>
       </c>
       <c r="AV30" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>292.11358799999994</v>
       </c>
       <c r="AW30" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1415.6273879999999</v>
       </c>
       <c r="AX30" t="s">
@@ -11405,7 +11516,7 @@
         <v>0</v>
       </c>
       <c r="BP30" s="6">
-        <f t="shared" ref="BP30:BP35" si="17">BN30*1.2</f>
+        <f t="shared" ref="BP30:BP35" si="18">BN30*1.2</f>
         <v>1363.629195</v>
       </c>
       <c r="BQ30" s="6">
@@ -11494,13 +11605,17 @@
       </c>
       <c r="CP30">
         <f t="shared" ca="1" si="14"/>
-        <v>0.45084860705225616</v>
+        <v>0.43140822736866213</v>
       </c>
       <c r="CQ30">
         <v>1</v>
       </c>
+      <c r="CR30" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1222603036</v>
       </c>
@@ -11649,11 +11764,11 @@
         <v>1424.3979960000001</v>
       </c>
       <c r="AV31" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>293.92339600000014</v>
       </c>
       <c r="AW31" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1424.3979960000001</v>
       </c>
       <c r="AX31" t="s">
@@ -11715,7 +11830,7 @@
         <v>0</v>
       </c>
       <c r="BP31" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1488.4801151999998</v>
       </c>
       <c r="BQ31" s="6">
@@ -11804,13 +11919,17 @@
       </c>
       <c r="CP31">
         <f t="shared" ca="1" si="14"/>
-        <v>0.4995696104240076</v>
+        <v>0.30407656206330047</v>
       </c>
       <c r="CQ31">
         <v>1</v>
       </c>
+      <c r="CR31" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1222603037</v>
       </c>
@@ -11959,11 +12078,11 @@
         <v>1026.3835199999999</v>
       </c>
       <c r="AV32" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>171.06391999999994</v>
       </c>
       <c r="AW32" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1026.3835199999999</v>
       </c>
       <c r="AX32" t="s">
@@ -12026,7 +12145,7 @@
         <v>0</v>
       </c>
       <c r="BP32" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1412.224506</v>
       </c>
       <c r="BQ32" s="6">
@@ -12115,10 +12234,14 @@
       </c>
       <c r="CP32">
         <f t="shared" ca="1" si="14"/>
-        <v>8.5698402006279428E-2</v>
+        <v>0.1105025289825875</v>
       </c>
       <c r="CQ32">
         <v>1</v>
+      </c>
+      <c r="CR32" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="33" spans="1:96" x14ac:dyDescent="0.35">
@@ -12334,7 +12457,7 @@
         <v>0</v>
       </c>
       <c r="BP33" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1817.5164983999996</v>
       </c>
       <c r="BQ33" s="6">
@@ -12423,12 +12546,15 @@
       </c>
       <c r="CP33">
         <f t="shared" ca="1" si="14"/>
-        <v>0.35500282983106024</v>
+        <v>0.53133167282023652</v>
       </c>
       <c r="CQ33">
         <v>1</v>
       </c>
-      <c r="CR33" s="11"/>
+      <c r="CR33" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
     <row r="34" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A34">
@@ -12462,7 +12588,7 @@
         <v>176</v>
       </c>
       <c r="K34" s="6">
-        <f t="shared" ref="K34:K57" si="18">AW34+BR34+CM34</f>
+        <f t="shared" ref="K34:K57" si="19">AW34+BR34+CM34</f>
         <v>3925.2565242000001</v>
       </c>
       <c r="L34" t="s">
@@ -12553,15 +12679,15 @@
         <v>2778.43</v>
       </c>
       <c r="AO34" s="6">
-        <f t="shared" ref="AO34:AO57" si="19">AM34*0.1</f>
+        <f t="shared" ref="AO34:AO57" si="20">AM34*0.1</f>
         <v>100.23400000000001</v>
       </c>
       <c r="AP34" s="6">
-        <f t="shared" ref="AP34:AP57" si="20">AM34*0.03</f>
+        <f t="shared" ref="AP34:AP57" si="21">AM34*0.03</f>
         <v>30.0702</v>
       </c>
       <c r="AQ34" s="6">
-        <f t="shared" ref="AQ34:AQ65" si="21">AM34+AO34+AP34</f>
+        <f t="shared" ref="AQ34:AQ57" si="22">AM34+AO34+AP34</f>
         <v>1132.6442000000002</v>
       </c>
       <c r="AR34">
@@ -12623,15 +12749,15 @@
         <v>2778.43</v>
       </c>
       <c r="BJ34" s="6">
-        <f t="shared" ref="BJ34:BJ57" si="22">BH34*0.1</f>
+        <f t="shared" ref="BJ34:BJ57" si="23">BH34*0.1</f>
         <v>101.82300000000001</v>
       </c>
       <c r="BK34" s="6">
-        <f t="shared" ref="BK34:BK57" si="23">BH34*0.03</f>
+        <f t="shared" ref="BK34:BK57" si="24">BH34*0.03</f>
         <v>30.546900000000001</v>
       </c>
       <c r="BL34" s="6">
-        <f t="shared" ref="BL34:BL65" si="24">BH34+BJ34+BK34</f>
+        <f t="shared" ref="BL34:BL57" si="25">BH34+BJ34+BK34</f>
         <v>1150.5999000000002</v>
       </c>
       <c r="BM34" s="6">
@@ -12645,15 +12771,15 @@
         <v>0</v>
       </c>
       <c r="BP34" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1470.4666722000002</v>
       </c>
       <c r="BQ34" s="6">
-        <f t="shared" ref="BQ34:BQ65" si="25">BP34-BL34</f>
+        <f t="shared" ref="BQ34:BQ57" si="26">BP34-BL34</f>
         <v>319.86677220000001</v>
       </c>
       <c r="BR34" s="6">
-        <f t="shared" ref="BR34:BR57" si="26">BP34</f>
+        <f t="shared" ref="BR34:BR57" si="27">BP34</f>
         <v>1470.4666722000002</v>
       </c>
       <c r="BS34" t="s">
@@ -12693,15 +12819,15 @@
         <v>2778.43</v>
       </c>
       <c r="CE34" s="6">
-        <f t="shared" ref="CE34:CE57" si="27">CC34*0.1</f>
+        <f t="shared" ref="CE34:CE57" si="28">CC34*0.1</f>
         <v>75.786000000000001</v>
       </c>
       <c r="CF34" s="6">
-        <f t="shared" ref="CF34:CF57" si="28">CC34*0.03</f>
+        <f t="shared" ref="CF34:CF57" si="29">CC34*0.03</f>
         <v>22.735800000000001</v>
       </c>
       <c r="CG34" s="6">
-        <f t="shared" ref="CG34:CG65" si="29">CC34+CE34+CF34</f>
+        <f t="shared" ref="CG34:CG57" si="30">CC34+CE34+CF34</f>
         <v>856.3818</v>
       </c>
       <c r="CH34" s="6">
@@ -12718,11 +12844,11 @@
         <v>1027.65816</v>
       </c>
       <c r="CL34" s="6">
-        <f t="shared" ref="CL34:CL65" si="30">CK34-CG34</f>
+        <f t="shared" ref="CL34:CL57" si="31">CK34-CG34</f>
         <v>171.27635999999995</v>
       </c>
       <c r="CM34" s="6">
-        <f t="shared" ref="CM34:CM57" si="31">CK34</f>
+        <f t="shared" ref="CM34:CM57" si="32">CK34</f>
         <v>1027.65816</v>
       </c>
       <c r="CN34" t="s">
@@ -12732,11 +12858,15 @@
         <v>477</v>
       </c>
       <c r="CP34">
-        <f t="shared" ref="CP34:CP57" ca="1" si="32">RAND()</f>
-        <v>0.49984354005007947</v>
+        <f t="shared" ref="CP34:CP57" ca="1" si="33">RAND()</f>
+        <v>0.29292242005083979</v>
       </c>
       <c r="CQ34">
         <v>1</v>
+      </c>
+      <c r="CR34" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="35" spans="1:96" x14ac:dyDescent="0.35">
@@ -12771,7 +12901,7 @@
         <v>176</v>
       </c>
       <c r="K35" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>38570.332081199995</v>
       </c>
       <c r="L35" t="s">
@@ -12863,15 +12993,15 @@
         <v>7352.1432000000004</v>
       </c>
       <c r="AO35" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>680.75400000000002</v>
       </c>
       <c r="AP35" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>204.22619999999998</v>
       </c>
       <c r="AQ35" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7692.5201999999999</v>
       </c>
       <c r="AR35">
@@ -12935,15 +13065,15 @@
         <v>6657.800400000001</v>
       </c>
       <c r="BJ35" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>616.46300000000008</v>
       </c>
       <c r="BK35" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>184.93889999999999</v>
       </c>
       <c r="BL35" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>6966.0319</v>
       </c>
       <c r="BM35" s="6">
@@ -12957,15 +13087,15 @@
         <v>0</v>
       </c>
       <c r="BP35" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8777.2001939999991</v>
       </c>
       <c r="BQ35" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1811.1682939999992</v>
       </c>
       <c r="BR35" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>8777.2001939999991</v>
       </c>
       <c r="BS35" t="s">
@@ -13006,15 +13136,15 @@
         <v>8337.999600000001</v>
       </c>
       <c r="CE35" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>772.03700000000003</v>
       </c>
       <c r="CF35" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>231.61109999999999</v>
       </c>
       <c r="CG35" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>8724.0180999999993</v>
       </c>
       <c r="CH35" s="6">
@@ -13032,11 +13162,11 @@
         <v>11515.703892</v>
       </c>
       <c r="CL35" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>2791.6857920000002</v>
       </c>
       <c r="CM35" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>11515.703892</v>
       </c>
       <c r="CN35" t="s">
@@ -13046,11 +13176,15 @@
         <v>264</v>
       </c>
       <c r="CP35">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.86619068814589395</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>6.9915721885898119E-3</v>
       </c>
       <c r="CQ35">
         <v>1</v>
+      </c>
+      <c r="CR35" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="36" spans="1:96" x14ac:dyDescent="0.35">
@@ -13085,7 +13219,7 @@
         <v>176</v>
       </c>
       <c r="K36" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3370.9346400000004</v>
       </c>
       <c r="L36" t="s">
@@ -13176,15 +13310,15 @@
         <v>2485.94</v>
       </c>
       <c r="AO36" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>95.157000000000011</v>
       </c>
       <c r="AP36" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>28.5471</v>
       </c>
       <c r="AQ36" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1075.2741000000001</v>
       </c>
       <c r="AR36">
@@ -13245,15 +13379,15 @@
         <v>2485.94</v>
       </c>
       <c r="BJ36" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>74.566999999999993</v>
       </c>
       <c r="BK36" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>22.370099999999997</v>
       </c>
       <c r="BL36" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>842.60709999999995</v>
       </c>
       <c r="BM36" s="6">
@@ -13270,11 +13404,11 @@
         <v>1011.1285199999999</v>
       </c>
       <c r="BQ36" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>168.52141999999992</v>
       </c>
       <c r="BR36" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1011.1285199999999</v>
       </c>
       <c r="BS36" t="s">
@@ -13314,15 +13448,15 @@
         <v>2485.94</v>
       </c>
       <c r="CE36" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>78.87</v>
       </c>
       <c r="CF36" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>23.661000000000001</v>
       </c>
       <c r="CG36" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>891.23099999999999</v>
       </c>
       <c r="CH36" s="6">
@@ -13339,11 +13473,11 @@
         <v>1069.4772</v>
       </c>
       <c r="CL36" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>178.24620000000004</v>
       </c>
       <c r="CM36" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1069.4772</v>
       </c>
       <c r="CN36" t="s">
@@ -13353,11 +13487,15 @@
         <v>187</v>
       </c>
       <c r="CP36">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.44106135782265288</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>6.5459961531728617E-2</v>
       </c>
       <c r="CQ36">
         <v>1</v>
+      </c>
+      <c r="CR36" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="37" spans="1:96" x14ac:dyDescent="0.35">
@@ -13392,7 +13530,7 @@
         <v>176</v>
       </c>
       <c r="K37" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5392.7970248000001</v>
       </c>
       <c r="L37" t="s">
@@ -13483,15 +13621,15 @@
         <v>3485.91</v>
       </c>
       <c r="AO37" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>129.46199999999999</v>
       </c>
       <c r="AP37" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>38.838599999999992</v>
       </c>
       <c r="AQ37" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1462.9205999999999</v>
       </c>
       <c r="AR37">
@@ -13551,15 +13689,15 @@
         <v>3485.91</v>
       </c>
       <c r="BJ37" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>134.167</v>
       </c>
       <c r="BK37" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>40.250100000000003</v>
       </c>
       <c r="BL37" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1516.0871</v>
       </c>
       <c r="BM37" s="6">
@@ -13577,11 +13715,11 @@
         <v>1855.6906104</v>
       </c>
       <c r="BQ37" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>339.6035104</v>
       </c>
       <c r="BR37" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1855.6906104</v>
       </c>
       <c r="BS37" t="s">
@@ -13621,15 +13759,15 @@
         <v>3485.91</v>
       </c>
       <c r="CE37" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>84.962000000000003</v>
       </c>
       <c r="CF37" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>25.488599999999998</v>
       </c>
       <c r="CG37" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>960.07060000000001</v>
       </c>
       <c r="CH37" s="6">
@@ -13647,11 +13785,11 @@
         <v>1175.1264143999999</v>
       </c>
       <c r="CL37" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>215.05581439999992</v>
       </c>
       <c r="CM37" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1175.1264143999999</v>
       </c>
       <c r="CN37" t="s">
@@ -13661,11 +13799,15 @@
         <v>310</v>
       </c>
       <c r="CP37">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.60578153244152322</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>4.2901923480578308E-2</v>
       </c>
       <c r="CQ37">
         <v>1</v>
+      </c>
+      <c r="CR37" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="38" spans="1:96" x14ac:dyDescent="0.35">
@@ -13700,7 +13842,7 @@
         <v>176</v>
       </c>
       <c r="K38" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5275.1601872000001</v>
       </c>
       <c r="L38" t="s">
@@ -13791,15 +13933,15 @@
         <v>3302.13</v>
       </c>
       <c r="AO38" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>111.70699999999999</v>
       </c>
       <c r="AP38" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33.512099999999997</v>
       </c>
       <c r="AQ38" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1262.2891</v>
       </c>
       <c r="AR38">
@@ -13859,15 +14001,15 @@
         <v>3302.13</v>
       </c>
       <c r="BJ38" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>105.76800000000001</v>
       </c>
       <c r="BK38" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>31.730399999999999</v>
       </c>
       <c r="BL38" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1195.1784</v>
       </c>
       <c r="BM38" s="6">
@@ -13885,11 +14027,11 @@
         <v>1462.8983615999998</v>
       </c>
       <c r="BQ38" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>267.71996159999981</v>
       </c>
       <c r="BR38" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1462.8983615999998</v>
       </c>
       <c r="BS38" t="s">
@@ -13929,15 +14071,15 @@
         <v>3302.13</v>
       </c>
       <c r="CE38" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>112.73800000000001</v>
       </c>
       <c r="CF38" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>33.821400000000004</v>
       </c>
       <c r="CG38" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1273.9394000000002</v>
       </c>
       <c r="CH38" s="6">
@@ -13955,11 +14097,11 @@
         <v>1559.3018256000003</v>
       </c>
       <c r="CL38" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>285.36242560000005</v>
       </c>
       <c r="CM38" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1559.3018256000003</v>
       </c>
       <c r="CN38" t="s">
@@ -13969,11 +14111,15 @@
         <v>452</v>
       </c>
       <c r="CP38">
-        <f t="shared" ca="1" si="32"/>
-        <v>4.9485300460342496E-2</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.91385261156435083</v>
       </c>
       <c r="CQ38">
         <v>1</v>
+      </c>
+      <c r="CR38" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="39" spans="1:96" x14ac:dyDescent="0.35">
@@ -14008,7 +14154,7 @@
         <v>176</v>
       </c>
       <c r="K39" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7656.7048499999992</v>
       </c>
       <c r="L39" t="s">
@@ -14099,15 +14245,15 @@
         <v>4673.97</v>
       </c>
       <c r="AO39" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>132.32599999999999</v>
       </c>
       <c r="AP39" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>39.697800000000001</v>
       </c>
       <c r="AQ39" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1495.2837999999999</v>
       </c>
       <c r="AR39">
@@ -14124,11 +14270,11 @@
         <v>1794.3405599999999</v>
       </c>
       <c r="AV39" s="6">
-        <f t="shared" ref="AV39:AV44" si="33">AU39-AQ39</f>
+        <f t="shared" ref="AV39:AV44" si="34">AU39-AQ39</f>
         <v>299.05675999999994</v>
       </c>
       <c r="AW39" s="6">
-        <f t="shared" ref="AW39:AW44" si="34">AU39</f>
+        <f t="shared" ref="AW39:AW44" si="35">AU39</f>
         <v>1794.3405599999999</v>
       </c>
       <c r="AX39" t="s">
@@ -14168,15 +14314,15 @@
         <v>4673.97</v>
       </c>
       <c r="BJ39" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>178.89600000000002</v>
       </c>
       <c r="BK39" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>53.668799999999997</v>
       </c>
       <c r="BL39" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2021.5247999999999</v>
       </c>
       <c r="BM39" s="6">
@@ -14194,11 +14340,11 @@
         <v>3638.7446399999994</v>
       </c>
       <c r="BQ39" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1617.2198399999995</v>
       </c>
       <c r="BR39" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3638.7446399999994</v>
       </c>
       <c r="BS39" t="s">
@@ -14238,15 +14384,15 @@
         <v>4673.97</v>
       </c>
       <c r="CE39" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>156.17500000000001</v>
       </c>
       <c r="CF39" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>46.852499999999999</v>
       </c>
       <c r="CG39" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1764.7774999999999</v>
       </c>
       <c r="CH39" s="6">
@@ -14264,11 +14410,11 @@
         <v>2223.6196499999996</v>
       </c>
       <c r="CL39" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>458.84214999999972</v>
       </c>
       <c r="CM39" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2223.6196499999996</v>
       </c>
       <c r="CN39" t="s">
@@ -14278,11 +14424,15 @@
         <v>489</v>
       </c>
       <c r="CP39">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.72877025317047806</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.23537634527222184</v>
       </c>
       <c r="CQ39">
         <v>1</v>
+      </c>
+      <c r="CR39" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="40" spans="1:96" x14ac:dyDescent="0.35">
@@ -14317,7 +14467,7 @@
         <v>98</v>
       </c>
       <c r="K40" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8722.7547599999998</v>
       </c>
       <c r="L40" t="s">
@@ -14409,15 +14559,15 @@
         <v>2118.4632000000001</v>
       </c>
       <c r="AO40" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>196.154</v>
       </c>
       <c r="AP40" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>58.846199999999996</v>
       </c>
       <c r="AQ40" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2216.5401999999999</v>
       </c>
       <c r="AR40">
@@ -14434,11 +14584,11 @@
         <v>2659.8482399999998</v>
       </c>
       <c r="AV40" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>443.30803999999989</v>
       </c>
       <c r="AW40" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>2659.8482399999998</v>
       </c>
       <c r="AX40" t="s">
@@ -14479,15 +14629,15 @@
         <v>1892.0520000000001</v>
       </c>
       <c r="BJ40" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>175.19000000000003</v>
       </c>
       <c r="BK40" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>52.557000000000002</v>
       </c>
       <c r="BL40" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1979.6470000000002</v>
       </c>
       <c r="BM40" s="6">
@@ -14505,11 +14655,11 @@
         <v>3563.3646000000003</v>
       </c>
       <c r="BQ40" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1583.7176000000002</v>
       </c>
       <c r="BR40" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3563.3646000000003</v>
       </c>
       <c r="BS40" t="s">
@@ -14550,15 +14700,15 @@
         <v>1990.7856000000002</v>
       </c>
       <c r="CE40" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>184.33199999999999</v>
       </c>
       <c r="CF40" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>55.299599999999998</v>
       </c>
       <c r="CG40" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2082.9515999999999</v>
       </c>
       <c r="CH40" s="6">
@@ -14575,11 +14725,11 @@
         <v>2499.5419199999997</v>
       </c>
       <c r="CL40" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>416.59031999999979</v>
       </c>
       <c r="CM40" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2499.5419199999997</v>
       </c>
       <c r="CN40" t="s">
@@ -14589,11 +14739,15 @@
         <v>403</v>
       </c>
       <c r="CP40">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.72650458086197067</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.84978275182471419</v>
       </c>
       <c r="CQ40">
         <v>1</v>
+      </c>
+      <c r="CR40" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="41" spans="1:96" x14ac:dyDescent="0.35">
@@ -14628,7 +14782,7 @@
         <v>98</v>
       </c>
       <c r="K41" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2194.8965189999999</v>
       </c>
       <c r="L41" t="s">
@@ -14720,15 +14874,15 @@
         <v>591.06240000000003</v>
       </c>
       <c r="AO41" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>54.728000000000002</v>
       </c>
       <c r="AP41" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>16.418399999999998</v>
       </c>
       <c r="AQ41" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>618.42639999999994</v>
       </c>
       <c r="AR41">
@@ -14745,11 +14899,11 @@
         <v>742.11167999999986</v>
       </c>
       <c r="AV41" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>123.68527999999992</v>
       </c>
       <c r="AW41" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>742.11167999999986</v>
       </c>
       <c r="AX41" t="s">
@@ -14790,15 +14944,15 @@
         <v>680.37840000000006</v>
       </c>
       <c r="BJ41" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>62.998000000000005</v>
       </c>
       <c r="BK41" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>18.8994</v>
       </c>
       <c r="BL41" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>711.87740000000008</v>
       </c>
       <c r="BM41" s="6">
@@ -14815,11 +14969,11 @@
         <v>854.25288000000012</v>
       </c>
       <c r="BQ41" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>142.37548000000004</v>
       </c>
       <c r="BR41" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>854.25288000000012</v>
       </c>
       <c r="BS41" t="s">
@@ -14860,15 +15014,15 @@
         <v>566.38440000000003</v>
       </c>
       <c r="CE41" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>52.442999999999998</v>
       </c>
       <c r="CF41" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.732899999999997</v>
       </c>
       <c r="CG41" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>592.60589999999991</v>
       </c>
       <c r="CH41" s="6">
@@ -14885,11 +15039,11 @@
         <v>598.53195899999992</v>
       </c>
       <c r="CL41" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>5.9260590000000093</v>
       </c>
       <c r="CM41" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>598.53195899999992</v>
       </c>
       <c r="CN41" t="s">
@@ -14899,11 +15053,15 @@
         <v>513</v>
       </c>
       <c r="CP41">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.41503075855102944</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.49338804146432524</v>
       </c>
       <c r="CQ41">
         <v>1</v>
+      </c>
+      <c r="CR41" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="42" spans="1:96" x14ac:dyDescent="0.35">
@@ -14938,7 +15096,7 @@
         <v>98</v>
       </c>
       <c r="K42" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1951.7450399999998</v>
       </c>
       <c r="L42" t="s">
@@ -15030,15 +15188,15 @@
         <v>486.31320000000005</v>
       </c>
       <c r="AO42" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>45.029000000000003</v>
       </c>
       <c r="AP42" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>13.508699999999999</v>
       </c>
       <c r="AQ42" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>508.82769999999999</v>
       </c>
       <c r="AR42">
@@ -15055,11 +15213,11 @@
         <v>610.59323999999992</v>
       </c>
       <c r="AV42" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>101.76553999999993</v>
       </c>
       <c r="AW42" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>610.59323999999992</v>
       </c>
       <c r="AX42" t="s">
@@ -15100,15 +15258,15 @@
         <v>544.47120000000007</v>
       </c>
       <c r="BJ42" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>50.414000000000001</v>
       </c>
       <c r="BK42" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>15.124199999999998</v>
       </c>
       <c r="BL42" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>569.67819999999995</v>
       </c>
       <c r="BM42" s="6">
@@ -15125,11 +15283,11 @@
         <v>683.61383999999987</v>
       </c>
       <c r="BQ42" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>113.93563999999992</v>
       </c>
       <c r="BR42" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>683.61383999999987</v>
       </c>
       <c r="BS42" t="s">
@@ -15170,15 +15328,15 @@
         <v>523.70280000000002</v>
       </c>
       <c r="CE42" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>48.491000000000007</v>
       </c>
       <c r="CF42" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>14.5473</v>
       </c>
       <c r="CG42" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>547.94830000000002</v>
       </c>
       <c r="CH42" s="6">
@@ -15195,11 +15353,11 @@
         <v>657.53796</v>
       </c>
       <c r="CL42" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>109.58965999999998</v>
       </c>
       <c r="CM42" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>657.53796</v>
       </c>
       <c r="CN42" t="s">
@@ -15209,11 +15367,15 @@
         <v>228</v>
       </c>
       <c r="CP42">
-        <f t="shared" ca="1" si="32"/>
-        <v>7.793011469631439E-2</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.76408569005543736</v>
       </c>
       <c r="CQ42">
         <v>1</v>
+      </c>
+      <c r="CR42" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="43" spans="1:96" x14ac:dyDescent="0.35">
@@ -15248,7 +15410,7 @@
         <v>98</v>
       </c>
       <c r="K43" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3320.4390305999996</v>
       </c>
       <c r="L43" t="s">
@@ -15340,15 +15502,15 @@
         <v>962.77680000000009</v>
       </c>
       <c r="AO43" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>89.146000000000015</v>
       </c>
       <c r="AP43" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>26.7438</v>
       </c>
       <c r="AQ43" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1007.3498</v>
       </c>
       <c r="AR43">
@@ -15365,11 +15527,11 @@
         <v>1208.8197599999999</v>
       </c>
       <c r="AV43" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>201.4699599999999</v>
       </c>
       <c r="AW43" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1208.8197599999999</v>
       </c>
       <c r="AX43" t="s">
@@ -15410,15 +15572,15 @@
         <v>813.01319999999998</v>
       </c>
       <c r="BJ43" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>75.278999999999996</v>
       </c>
       <c r="BK43" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>22.583699999999997</v>
       </c>
       <c r="BL43" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>850.65269999999998</v>
       </c>
       <c r="BM43" s="6">
@@ -15436,11 +15598,11 @@
         <v>1087.1341505999999</v>
       </c>
       <c r="BQ43" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>236.4814505999999</v>
       </c>
       <c r="BR43" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1087.1341505999999</v>
       </c>
       <c r="BS43" t="s">
@@ -15481,15 +15643,15 @@
         <v>815.96160000000009</v>
       </c>
       <c r="CE43" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>75.552000000000007</v>
       </c>
       <c r="CF43" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>22.665599999999998</v>
       </c>
       <c r="CG43" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>853.73760000000004</v>
       </c>
       <c r="CH43" s="6">
@@ -15506,11 +15668,11 @@
         <v>1024.4851200000001</v>
       </c>
       <c r="CL43" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>170.74752000000001</v>
       </c>
       <c r="CM43" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1024.4851200000001</v>
       </c>
       <c r="CN43" t="s">
@@ -15520,11 +15682,15 @@
         <v>519</v>
       </c>
       <c r="CP43">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.38324190857005747</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.55038181498423533</v>
       </c>
       <c r="CQ43">
         <v>1</v>
+      </c>
+      <c r="CR43" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="44" spans="1:96" x14ac:dyDescent="0.35">
@@ -15559,7 +15725,7 @@
         <v>176</v>
       </c>
       <c r="K44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2588.8286439999997</v>
       </c>
       <c r="L44" t="s">
@@ -15650,15 +15816,15 @@
         <v>1939.38</v>
       </c>
       <c r="AO44" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>67.641999999999996</v>
       </c>
       <c r="AP44" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>20.292599999999997</v>
       </c>
       <c r="AQ44" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>764.35459999999989</v>
       </c>
       <c r="AR44">
@@ -15676,11 +15842,11 @@
         <v>1008.9480719999999</v>
       </c>
       <c r="AV44" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>244.59347200000002</v>
       </c>
       <c r="AW44" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1008.9480719999999</v>
       </c>
       <c r="AX44" t="s">
@@ -15720,15 +15886,15 @@
         <v>1939.38</v>
       </c>
       <c r="BJ44" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>64.492000000000004</v>
       </c>
       <c r="BK44" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>19.347599999999996</v>
       </c>
       <c r="BL44" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>728.75959999999986</v>
       </c>
       <c r="BM44" s="6">
@@ -15745,11 +15911,11 @@
         <v>874.51151999999979</v>
       </c>
       <c r="BQ44" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>145.75191999999993</v>
       </c>
       <c r="BR44" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>874.51151999999979</v>
       </c>
       <c r="BS44" t="s">
@@ -15789,15 +15955,15 @@
         <v>1939.38</v>
       </c>
       <c r="CE44" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>61.804000000000002</v>
       </c>
       <c r="CF44" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>18.5412</v>
       </c>
       <c r="CG44" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>698.38519999999994</v>
       </c>
       <c r="CH44" s="6">
@@ -15814,11 +15980,11 @@
         <v>705.3690519999999</v>
       </c>
       <c r="CL44" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>6.9838519999999562</v>
       </c>
       <c r="CM44" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>705.3690519999999</v>
       </c>
       <c r="CN44" t="s">
@@ -15828,11 +15994,15 @@
         <v>337</v>
       </c>
       <c r="CP44">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.18533196817809039</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.42462531715704355</v>
       </c>
       <c r="CQ44">
         <v>1</v>
+      </c>
+      <c r="CR44" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="45" spans="1:96" x14ac:dyDescent="0.35">
@@ -15867,7 +16037,7 @@
         <v>98</v>
       </c>
       <c r="K45" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7444.6051935999994</v>
       </c>
       <c r="L45" t="s">
@@ -15959,15 +16129,15 @@
         <v>949.62240000000008</v>
       </c>
       <c r="AO45" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>87.927999999999997</v>
       </c>
       <c r="AP45" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>26.378399999999999</v>
       </c>
       <c r="AQ45" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>993.58639999999991</v>
       </c>
       <c r="AR45">
@@ -16027,15 +16197,15 @@
         <v>1046.0340000000001</v>
       </c>
       <c r="BJ45" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>96.855000000000004</v>
       </c>
       <c r="BK45" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>29.056499999999996</v>
       </c>
       <c r="BL45" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1094.4614999999999</v>
       </c>
       <c r="BM45" s="6">
@@ -16053,11 +16223,11 @@
         <v>1339.6208759999997</v>
       </c>
       <c r="BQ45" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>245.15937599999984</v>
       </c>
       <c r="BR45" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1339.6208759999997</v>
       </c>
       <c r="BS45" t="s">
@@ -16098,15 +16268,15 @@
         <v>1428.5484000000001</v>
       </c>
       <c r="CE45" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>132.273</v>
       </c>
       <c r="CF45" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>39.681899999999999</v>
       </c>
       <c r="CG45" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1494.6849</v>
       </c>
       <c r="CH45" s="6">
@@ -16124,11 +16294,11 @@
         <v>1829.4943175999999</v>
       </c>
       <c r="CL45" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>334.80941759999996</v>
       </c>
       <c r="CM45" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1829.4943175999999</v>
       </c>
       <c r="CN45" t="s">
@@ -16138,11 +16308,15 @@
         <v>172</v>
       </c>
       <c r="CP45">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.74317582227670675</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.43167936556886743</v>
       </c>
       <c r="CQ45">
         <v>1</v>
+      </c>
+      <c r="CR45" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="46" spans="1:96" x14ac:dyDescent="0.35">
@@ -16177,7 +16351,7 @@
         <v>98</v>
       </c>
       <c r="K46" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7631.7917399999997</v>
       </c>
       <c r="L46" t="s">
@@ -16269,15 +16443,15 @@
         <v>1671.3000000000002</v>
       </c>
       <c r="AO46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>154.75</v>
       </c>
       <c r="AP46" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>46.424999999999997</v>
       </c>
       <c r="AQ46" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1748.675</v>
       </c>
       <c r="AR46">
@@ -16294,11 +16468,11 @@
         <v>2098.41</v>
       </c>
       <c r="AV46" s="6">
-        <f t="shared" ref="AV46:AV52" si="35">AU46-AQ46</f>
+        <f t="shared" ref="AV46:AV52" si="36">AU46-AQ46</f>
         <v>349.7349999999999</v>
       </c>
       <c r="AW46" s="6">
-        <f t="shared" ref="AW46:AW52" si="36">AU46</f>
+        <f t="shared" ref="AW46:AW52" si="37">AU46</f>
         <v>2098.41</v>
       </c>
       <c r="AX46" t="s">
@@ -16339,15 +16513,15 @@
         <v>1835.838</v>
       </c>
       <c r="BJ46" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>169.98500000000001</v>
       </c>
       <c r="BK46" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>50.995499999999993</v>
       </c>
       <c r="BL46" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1920.8305</v>
       </c>
       <c r="BM46" s="6">
@@ -16365,11 +16539,11 @@
         <v>3457.4949000000001</v>
       </c>
       <c r="BQ46" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1536.6644000000001</v>
       </c>
       <c r="BR46" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3457.4949000000001</v>
       </c>
       <c r="BS46" t="s">
@@ -16410,15 +16584,15 @@
         <v>1653.3612000000003</v>
       </c>
       <c r="CE46" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>153.08900000000003</v>
       </c>
       <c r="CF46" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>45.926700000000004</v>
       </c>
       <c r="CG46" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1729.9057</v>
       </c>
       <c r="CH46" s="6">
@@ -16435,11 +16609,11 @@
         <v>2075.8868400000001</v>
       </c>
       <c r="CL46" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>345.9811400000001</v>
       </c>
       <c r="CM46" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2075.8868400000001</v>
       </c>
       <c r="CN46" t="s">
@@ -16449,11 +16623,15 @@
         <v>237</v>
       </c>
       <c r="CP46">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.82746694762164408</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.53301151181363393</v>
       </c>
       <c r="CQ46">
         <v>1</v>
+      </c>
+      <c r="CR46" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="47" spans="1:96" x14ac:dyDescent="0.35">
@@ -16488,7 +16666,7 @@
         <v>176</v>
       </c>
       <c r="K47" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2646.9235260000005</v>
       </c>
       <c r="L47" t="s">
@@ -16579,15 +16757,15 @@
         <v>1983.96</v>
       </c>
       <c r="AO47" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>61.595000000000006</v>
       </c>
       <c r="AP47" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>18.4785</v>
       </c>
       <c r="AQ47" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>696.02350000000013</v>
       </c>
       <c r="AR47">
@@ -16605,11 +16783,11 @@
         <v>918.75102000000027</v>
       </c>
       <c r="AV47" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>222.72752000000014</v>
       </c>
       <c r="AW47" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>918.75102000000027</v>
       </c>
       <c r="AX47" t="s">
@@ -16649,15 +16827,15 @@
         <v>1983.96</v>
       </c>
       <c r="BJ47" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>77.719000000000008</v>
       </c>
       <c r="BK47" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>23.3157</v>
       </c>
       <c r="BL47" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>878.2247000000001</v>
       </c>
       <c r="BM47" s="6">
@@ -16674,11 +16852,11 @@
         <v>1053.8696400000001</v>
       </c>
       <c r="BQ47" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>175.64494000000002</v>
       </c>
       <c r="BR47" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1053.8696400000001</v>
       </c>
       <c r="BS47" t="s">
@@ -16718,15 +16896,15 @@
         <v>1983.96</v>
       </c>
       <c r="CE47" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>59.082000000000008</v>
       </c>
       <c r="CF47" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>17.724600000000002</v>
       </c>
       <c r="CG47" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>667.62660000000005</v>
       </c>
       <c r="CH47" s="6">
@@ -16743,11 +16921,11 @@
         <v>674.30286600000011</v>
       </c>
       <c r="CL47" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>6.6762660000000551</v>
       </c>
       <c r="CM47" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>674.30286600000011</v>
       </c>
       <c r="CN47" t="s">
@@ -16757,11 +16935,15 @@
         <v>428</v>
       </c>
       <c r="CP47">
-        <f t="shared" ca="1" si="32"/>
-        <v>1.3165593692000543E-3</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.873169751956277</v>
       </c>
       <c r="CQ47">
         <v>1</v>
+      </c>
+      <c r="CR47" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
     <row r="48" spans="1:96" x14ac:dyDescent="0.35">
@@ -16796,7 +16978,7 @@
         <v>176</v>
       </c>
       <c r="K48" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6569.1006419999994</v>
       </c>
       <c r="L48" t="s">
@@ -16888,15 +17070,15 @@
         <v>1875.9168000000002</v>
       </c>
       <c r="AO48" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>173.69600000000003</v>
       </c>
       <c r="AP48" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>52.108800000000002</v>
       </c>
       <c r="AQ48" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1962.7647999999999</v>
       </c>
       <c r="AR48">
@@ -16913,11 +17095,11 @@
         <v>2355.3177599999999</v>
       </c>
       <c r="AV48" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>392.55295999999998</v>
       </c>
       <c r="AW48" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2355.3177599999999</v>
       </c>
       <c r="AX48" t="s">
@@ -16958,15 +17140,15 @@
         <v>1438.6248000000001</v>
       </c>
       <c r="BJ48" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>133.20599999999999</v>
       </c>
       <c r="BK48" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>39.961799999999997</v>
       </c>
       <c r="BL48" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1505.2277999999999</v>
       </c>
       <c r="BM48" s="6">
@@ -16984,11 +17166,11 @@
         <v>2709.4100399999998</v>
       </c>
       <c r="BQ48" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1204.1822399999999</v>
       </c>
       <c r="BR48" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2709.4100399999998</v>
       </c>
       <c r="BS48" t="s">
@@ -17029,15 +17211,15 @@
         <v>1141.1171999999999</v>
       </c>
       <c r="CE48" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>105.65899999999999</v>
       </c>
       <c r="CF48" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>31.697699999999998</v>
       </c>
       <c r="CG48" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1193.9466999999997</v>
       </c>
       <c r="CH48" s="6">
@@ -17055,11 +17237,11 @@
         <v>1504.3728419999998</v>
       </c>
       <c r="CL48" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>310.42614200000003</v>
       </c>
       <c r="CM48" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1504.3728419999998</v>
       </c>
       <c r="CN48" t="s">
@@ -17069,14 +17251,18 @@
         <v>446</v>
       </c>
       <c r="CP48">
-        <f t="shared" ca="1" si="32"/>
-        <v>2.1048901883236049E-4</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.95377368627295533</v>
       </c>
       <c r="CQ48">
         <v>1</v>
       </c>
+      <c r="CR48" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="49" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1222603057</v>
       </c>
@@ -17108,7 +17294,7 @@
         <v>176</v>
       </c>
       <c r="K49" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1879.3606752000001</v>
       </c>
       <c r="L49" t="s">
@@ -17199,15 +17385,15 @@
         <v>1251.04</v>
       </c>
       <c r="AO49" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30.3</v>
       </c>
       <c r="AP49" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9.09</v>
       </c>
       <c r="AQ49" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>342.39</v>
       </c>
       <c r="AR49">
@@ -17225,11 +17411,11 @@
         <v>460.17216000000002</v>
       </c>
       <c r="AV49" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>117.78216000000003</v>
       </c>
       <c r="AW49" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>460.17216000000002</v>
       </c>
       <c r="AX49" t="s">
@@ -17269,15 +17455,15 @@
         <v>1251.04</v>
       </c>
       <c r="BJ49" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>56.79</v>
       </c>
       <c r="BK49" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>17.036999999999999</v>
       </c>
       <c r="BL49" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>641.72699999999998</v>
       </c>
       <c r="BM49" s="6">
@@ -17295,11 +17481,11 @@
         <v>862.481088</v>
       </c>
       <c r="BQ49" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>220.75408800000002</v>
       </c>
       <c r="BR49" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>862.481088</v>
       </c>
       <c r="BS49" t="s">
@@ -17339,15 +17525,15 @@
         <v>1251.04</v>
       </c>
       <c r="CE49" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>38.014000000000003</v>
       </c>
       <c r="CF49" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>11.404199999999999</v>
       </c>
       <c r="CG49" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>429.5582</v>
       </c>
       <c r="CH49" s="6">
@@ -17365,11 +17551,11 @@
         <v>556.70742719999998</v>
       </c>
       <c r="CL49" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>127.14922719999998</v>
       </c>
       <c r="CM49" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>556.70742719999998</v>
       </c>
       <c r="CN49" t="s">
@@ -17379,14 +17565,18 @@
         <v>483</v>
       </c>
       <c r="CP49">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.38294061423868186</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.68471666147565347</v>
       </c>
       <c r="CQ49">
         <v>1</v>
       </c>
+      <c r="CR49" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="50" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1222603058</v>
       </c>
@@ -17418,7 +17608,7 @@
         <v>176</v>
       </c>
       <c r="K50" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4364.0011044000003</v>
       </c>
       <c r="L50" t="s">
@@ -17509,15 +17699,15 @@
         <v>3048.1</v>
       </c>
       <c r="AO50" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>87.563000000000002</v>
       </c>
       <c r="AP50" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>26.268899999999999</v>
       </c>
       <c r="AQ50" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>989.46190000000001</v>
       </c>
       <c r="AR50">
@@ -17535,11 +17725,11 @@
         <v>1246.721994</v>
       </c>
       <c r="AV50" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>257.26009399999998</v>
       </c>
       <c r="AW50" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1246.721994</v>
       </c>
       <c r="AX50" t="s">
@@ -17579,15 +17769,15 @@
         <v>3048.1</v>
       </c>
       <c r="BJ50" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>118.47300000000001</v>
       </c>
       <c r="BK50" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>35.541899999999998</v>
       </c>
       <c r="BL50" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1338.7448999999999</v>
       </c>
       <c r="BM50" s="6">
@@ -17605,11 +17795,11 @@
         <v>1670.7536352</v>
       </c>
       <c r="BQ50" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>332.00873520000005</v>
       </c>
       <c r="BR50" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1670.7536352</v>
       </c>
       <c r="BS50" t="s">
@@ -17649,15 +17839,15 @@
         <v>3048.1</v>
       </c>
       <c r="CE50" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>98.774000000000001</v>
       </c>
       <c r="CF50" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>29.632199999999997</v>
       </c>
       <c r="CG50" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1116.1462000000001</v>
       </c>
       <c r="CH50" s="6">
@@ -17675,11 +17865,11 @@
         <v>1446.5254752000001</v>
       </c>
       <c r="CL50" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>330.37927519999994</v>
       </c>
       <c r="CM50" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1446.5254752000001</v>
       </c>
       <c r="CN50" t="s">
@@ -17689,14 +17879,18 @@
         <v>458</v>
       </c>
       <c r="CP50">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.34708019432895865</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.69590792719270356</v>
       </c>
       <c r="CQ50">
         <v>1</v>
       </c>
+      <c r="CR50" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="51" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1222603059</v>
       </c>
@@ -17728,7 +17922,7 @@
         <v>176</v>
       </c>
       <c r="K51" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4310.9457060000004</v>
       </c>
       <c r="L51" t="s">
@@ -17820,15 +18014,15 @@
         <v>1131.0084000000002</v>
       </c>
       <c r="AO51" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>104.72300000000001</v>
       </c>
       <c r="AP51" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>31.416899999999998</v>
       </c>
       <c r="AQ51" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1183.3698999999999</v>
       </c>
       <c r="AR51">
@@ -17846,11 +18040,11 @@
         <v>1491.0460740000001</v>
       </c>
       <c r="AV51" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>307.67617400000017</v>
       </c>
       <c r="AW51" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1491.0460740000001</v>
       </c>
       <c r="AX51" t="s">
@@ -17891,15 +18085,15 @@
         <v>1041.3144</v>
       </c>
       <c r="BJ51" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>96.418000000000006</v>
       </c>
       <c r="BK51" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>28.925399999999996</v>
       </c>
       <c r="BL51" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1089.5234</v>
       </c>
       <c r="BM51" s="6">
@@ -17917,11 +18111,11 @@
         <v>1359.7252032000001</v>
       </c>
       <c r="BQ51" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>270.20180320000009</v>
       </c>
       <c r="BR51" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1359.7252032000001</v>
       </c>
       <c r="BS51" t="s">
@@ -17962,15 +18156,15 @@
         <v>1076.8248000000001</v>
       </c>
       <c r="CE51" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>99.706000000000003</v>
       </c>
       <c r="CF51" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>29.911799999999996</v>
       </c>
       <c r="CG51" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1126.6777999999999</v>
       </c>
       <c r="CH51" s="6">
@@ -17988,11 +18182,11 @@
         <v>1460.1744288</v>
       </c>
       <c r="CL51" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>333.49662880000005</v>
       </c>
       <c r="CM51" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1460.1744288</v>
       </c>
       <c r="CN51" t="s">
@@ -18002,14 +18196,18 @@
         <v>255</v>
       </c>
       <c r="CP51">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.12136058384629844</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.89584070138083649</v>
       </c>
       <c r="CQ51">
         <v>1</v>
       </c>
+      <c r="CR51" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="52" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1222603060</v>
       </c>
@@ -18041,7 +18239,7 @@
         <v>98</v>
       </c>
       <c r="K52" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3988.8502799999997</v>
       </c>
       <c r="L52" t="s">
@@ -18133,15 +18331,15 @@
         <v>1187.1792</v>
       </c>
       <c r="AO52" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>109.92400000000001</v>
       </c>
       <c r="AP52" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>32.977199999999996</v>
       </c>
       <c r="AQ52" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1242.1412</v>
       </c>
       <c r="AR52">
@@ -18158,11 +18356,11 @@
         <v>1490.56944</v>
       </c>
       <c r="AV52" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>248.42823999999996</v>
       </c>
       <c r="AW52" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1490.56944</v>
       </c>
       <c r="AX52" t="s">
@@ -18203,15 +18401,15 @@
         <v>823.05720000000008</v>
       </c>
       <c r="BJ52" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>76.209000000000003</v>
       </c>
       <c r="BK52" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>22.8627</v>
       </c>
       <c r="BL52" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>861.1617</v>
       </c>
       <c r="BM52" s="6">
@@ -18228,11 +18426,11 @@
         <v>1033.3940399999999</v>
       </c>
       <c r="BQ52" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>172.23233999999991</v>
       </c>
       <c r="BR52" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1033.3940399999999</v>
       </c>
       <c r="BS52" t="s">
@@ -18273,15 +18471,15 @@
         <v>1166.7239999999999</v>
       </c>
       <c r="CE52" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>108.03</v>
       </c>
       <c r="CF52" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>32.408999999999999</v>
       </c>
       <c r="CG52" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1220.739</v>
       </c>
       <c r="CH52" s="6">
@@ -18298,11 +18496,11 @@
         <v>1464.8868</v>
       </c>
       <c r="CL52" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>244.14779999999996</v>
       </c>
       <c r="CM52" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1464.8868</v>
       </c>
       <c r="CN52" t="s">
@@ -18312,14 +18510,18 @@
         <v>373</v>
       </c>
       <c r="CP52">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.84744823897055033</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>3.0658586560611822E-2</v>
       </c>
       <c r="CQ52">
         <v>1</v>
       </c>
+      <c r="CR52" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="53" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1222603061</v>
       </c>
@@ -18351,7 +18553,7 @@
         <v>176</v>
       </c>
       <c r="K53" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5936.0085159999999</v>
       </c>
       <c r="L53" t="s">
@@ -18442,15 +18644,15 @@
         <v>4203.6899999999996</v>
       </c>
       <c r="AO53" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>132.56400000000002</v>
       </c>
       <c r="AP53" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>39.769200000000005</v>
       </c>
       <c r="AQ53" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1497.9732000000001</v>
       </c>
       <c r="AR53">
@@ -18510,15 +18712,15 @@
         <v>4203.6899999999996</v>
       </c>
       <c r="BJ53" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>143.19200000000001</v>
       </c>
       <c r="BK53" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>42.957599999999999</v>
       </c>
       <c r="BL53" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1618.0696</v>
       </c>
       <c r="BM53" s="6">
@@ -18536,11 +18738,11 @@
         <v>1980.5171903999999</v>
       </c>
       <c r="BQ53" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>362.44759039999985</v>
       </c>
       <c r="BR53" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1980.5171903999999</v>
       </c>
       <c r="BS53" t="s">
@@ -18580,15 +18782,15 @@
         <v>4203.6899999999996</v>
       </c>
       <c r="CE53" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>144.61300000000003</v>
       </c>
       <c r="CF53" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>43.383900000000004</v>
       </c>
       <c r="CG53" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1634.1269000000002</v>
       </c>
       <c r="CH53" s="6">
@@ -18606,11 +18808,11 @@
         <v>2000.1713256000003</v>
       </c>
       <c r="CL53" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>366.04442560000007</v>
       </c>
       <c r="CM53" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2000.1713256000003</v>
       </c>
       <c r="CN53" t="s">
@@ -18620,14 +18822,18 @@
         <v>246</v>
       </c>
       <c r="CP53">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.44902108421063514</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.6301503474860447</v>
       </c>
       <c r="CQ53">
         <v>1</v>
       </c>
+      <c r="CR53" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="54" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1222603062</v>
       </c>
@@ -18659,7 +18865,7 @@
         <v>98</v>
       </c>
       <c r="K54" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5991.5194351999999</v>
       </c>
       <c r="L54" t="s">
@@ -18751,15 +18957,15 @@
         <v>1020.4164000000001</v>
       </c>
       <c r="AO54" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>94.483000000000004</v>
       </c>
       <c r="AP54" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>28.344899999999999</v>
       </c>
       <c r="AQ54" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1067.6579000000002</v>
       </c>
       <c r="AR54">
@@ -18819,15 +19025,15 @@
         <v>919.11239999999998</v>
       </c>
       <c r="BJ54" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>85.103000000000009</v>
       </c>
       <c r="BK54" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>25.530899999999999</v>
       </c>
       <c r="BL54" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>961.66390000000001</v>
       </c>
       <c r="BM54" s="6">
@@ -18845,11 +19051,11 @@
         <v>1177.0766136</v>
       </c>
       <c r="BQ54" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>215.41271359999996</v>
       </c>
       <c r="BR54" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1177.0766136</v>
       </c>
       <c r="BS54" t="s">
@@ -18890,15 +19096,15 @@
         <v>955.18439999999998</v>
       </c>
       <c r="CE54" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>88.442999999999998</v>
       </c>
       <c r="CF54" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>26.532899999999998</v>
       </c>
       <c r="CG54" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>999.40589999999997</v>
       </c>
       <c r="CH54" s="6">
@@ -18916,11 +19122,11 @@
         <v>1223.2728215999998</v>
       </c>
       <c r="CL54" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>223.86692159999984</v>
       </c>
       <c r="CM54" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1223.2728215999998</v>
       </c>
       <c r="CN54" t="s">
@@ -18930,14 +19136,18 @@
         <v>367</v>
       </c>
       <c r="CP54">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.16625761609607714</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.77024615409248742</v>
       </c>
       <c r="CQ54">
         <v>1</v>
       </c>
+      <c r="CR54" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="55" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1222603064</v>
       </c>
@@ -18969,7 +19179,7 @@
         <v>98</v>
       </c>
       <c r="K55" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7153.4898599999997</v>
       </c>
       <c r="L55" t="s">
@@ -19061,15 +19271,15 @@
         <v>1813.4064000000001</v>
       </c>
       <c r="AO55" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>167.90800000000002</v>
       </c>
       <c r="AP55" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>50.372399999999999</v>
       </c>
       <c r="AQ55" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1897.3603999999998</v>
       </c>
       <c r="AR55">
@@ -19131,15 +19341,15 @@
         <v>1179.6300000000001</v>
       </c>
       <c r="BJ55" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>109.22500000000001</v>
       </c>
       <c r="BK55" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>32.767499999999998</v>
       </c>
       <c r="BL55" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1234.2424999999998</v>
       </c>
       <c r="BM55" s="6">
@@ -19157,11 +19367,11 @@
         <v>2221.6364999999996</v>
       </c>
       <c r="BQ55" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>987.39399999999978</v>
       </c>
       <c r="BR55" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2221.6364999999996</v>
       </c>
       <c r="BS55" t="s">
@@ -19202,15 +19412,15 @@
         <v>2114.6184000000003</v>
       </c>
       <c r="CE55" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>195.798</v>
       </c>
       <c r="CF55" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>58.739399999999996</v>
       </c>
       <c r="CG55" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2212.5174000000002</v>
       </c>
       <c r="CH55" s="6">
@@ -19227,11 +19437,11 @@
         <v>2655.02088</v>
       </c>
       <c r="CL55" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>442.50347999999985</v>
       </c>
       <c r="CM55" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2655.02088</v>
       </c>
       <c r="CN55" t="s">
@@ -19241,14 +19451,18 @@
         <v>531</v>
       </c>
       <c r="CP55">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.23131549983717747</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.37256229732460289</v>
       </c>
       <c r="CQ55">
         <v>1</v>
       </c>
+      <c r="CR55" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="56" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1222603601</v>
       </c>
@@ -19280,7 +19494,7 @@
         <v>98</v>
       </c>
       <c r="K56" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>30090.770904000001</v>
       </c>
       <c r="L56" t="s">
@@ -19372,15 +19586,15 @@
         <v>7121.7683999999999</v>
       </c>
       <c r="AO56" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>659.423</v>
       </c>
       <c r="AP56" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>197.82689999999997</v>
       </c>
       <c r="AQ56" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7451.4798999999994</v>
       </c>
       <c r="AR56">
@@ -19443,15 +19657,15 @@
         <v>5708.9340000000002</v>
       </c>
       <c r="BJ56" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>528.60500000000002</v>
       </c>
       <c r="BK56" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>158.58150000000001</v>
       </c>
       <c r="BL56" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5973.2365000000009</v>
       </c>
       <c r="BM56" s="6">
@@ -19468,11 +19682,11 @@
         <v>7167.8838000000005</v>
       </c>
       <c r="BQ56" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1194.6472999999996</v>
       </c>
       <c r="BR56" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>7167.8838000000005</v>
       </c>
       <c r="BS56" t="s">
@@ -19513,15 +19727,15 @@
         <v>5437.9836000000005</v>
       </c>
       <c r="CE56" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>503.51700000000005</v>
       </c>
       <c r="CF56" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>151.05510000000001</v>
       </c>
       <c r="CG56" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>5689.7420999999995</v>
       </c>
       <c r="CH56" s="6">
@@ -19538,11 +19752,11 @@
         <v>6827.6905199999992</v>
       </c>
       <c r="CL56" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1137.9484199999997</v>
       </c>
       <c r="CM56" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>6827.6905199999992</v>
       </c>
       <c r="CN56" t="s">
@@ -19552,14 +19766,18 @@
         <v>507</v>
       </c>
       <c r="CP56">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.65476860444207319</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.50649833381527587</v>
       </c>
       <c r="CQ56">
         <v>1</v>
       </c>
+      <c r="CR56" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
+      </c>
     </row>
-    <row r="57" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:96" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1232603801</v>
       </c>
@@ -19591,7 +19809,7 @@
         <v>176</v>
       </c>
       <c r="K57" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2643.1632250000002</v>
       </c>
       <c r="L57" t="s">
@@ -19682,15 +19900,15 @@
         <v>1965.17</v>
       </c>
       <c r="AO57" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>76.463999999999999</v>
       </c>
       <c r="AP57" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>22.9392</v>
       </c>
       <c r="AQ57" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>864.04320000000007</v>
       </c>
       <c r="AR57">
@@ -19752,15 +19970,15 @@
         <v>1965.17</v>
       </c>
       <c r="BJ57" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>61.696000000000005</v>
       </c>
       <c r="BK57" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>18.508800000000001</v>
       </c>
       <c r="BL57" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>697.16480000000001</v>
       </c>
       <c r="BM57" s="6">
@@ -19777,11 +19995,11 @@
         <v>836.59775999999999</v>
       </c>
       <c r="BQ57" s="6">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>139.43295999999998</v>
       </c>
       <c r="BR57" s="6">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>836.59775999999999</v>
       </c>
       <c r="BS57" t="s">
@@ -19821,15 +20039,15 @@
         <v>1965.17</v>
       </c>
       <c r="CE57" s="6">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>58.357000000000006</v>
       </c>
       <c r="CF57" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>17.507100000000001</v>
       </c>
       <c r="CG57" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>659.43410000000006</v>
       </c>
       <c r="CH57" s="6">
@@ -19846,11 +20064,11 @@
         <v>666.02844100000004</v>
       </c>
       <c r="CL57" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>6.5943409999999858</v>
       </c>
       <c r="CM57" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>666.02844100000004</v>
       </c>
       <c r="CN57" t="s">
@@ -19860,11 +20078,15 @@
         <v>471</v>
       </c>
       <c r="CP57">
-        <f t="shared" ca="1" si="32"/>
-        <v>0.23795730018813543</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>0.46863257963331673</v>
       </c>
       <c r="CQ57">
         <v>1</v>
+      </c>
+      <c r="CR57" s="10" t="str">
+        <f t="shared" si="15"/>
+        <v>20.12.2025 22:00</v>
       </c>
     </row>
   </sheetData>
@@ -21054,7 +21276,7 @@
       </c>
       <c r="CP2">
         <f t="shared" ref="CP2:CP57" ca="1" si="14">RAND()</f>
-        <v>0.62016037330583607</v>
+        <v>0.2113128188617841</v>
       </c>
       <c r="CR2" s="10"/>
     </row>
@@ -21363,7 +21585,7 @@
       </c>
       <c r="CP3">
         <f t="shared" ca="1" si="14"/>
-        <v>0.81012137936216533</v>
+        <v>0.71777867012039476</v>
       </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.35">
@@ -21667,7 +21889,7 @@
       </c>
       <c r="CP4">
         <f t="shared" ca="1" si="14"/>
-        <v>0.62460094294933122</v>
+        <v>0.87979596127737814</v>
       </c>
     </row>
     <row r="5" spans="1:97" x14ac:dyDescent="0.35">
@@ -21974,7 +22196,7 @@
       </c>
       <c r="CP5">
         <f t="shared" ca="1" si="14"/>
-        <v>0.4485680367397995</v>
+        <v>0.27044460173440199</v>
       </c>
     </row>
     <row r="6" spans="1:97" x14ac:dyDescent="0.35">
@@ -22281,7 +22503,7 @@
       </c>
       <c r="CP6">
         <f t="shared" ca="1" si="14"/>
-        <v>0.14212829921057302</v>
+        <v>0.66254617717869502</v>
       </c>
     </row>
     <row r="7" spans="1:97" x14ac:dyDescent="0.35">
@@ -22589,7 +22811,7 @@
       </c>
       <c r="CP7">
         <f t="shared" ca="1" si="14"/>
-        <v>0.33001123977306612</v>
+        <v>8.9262331730229794E-2</v>
       </c>
     </row>
     <row r="8" spans="1:97" x14ac:dyDescent="0.35">
@@ -22896,7 +23118,7 @@
       </c>
       <c r="CP8">
         <f t="shared" ca="1" si="14"/>
-        <v>2.7713057968083987E-2</v>
+        <v>0.62583464989212867</v>
       </c>
     </row>
     <row r="9" spans="1:97" x14ac:dyDescent="0.35">
@@ -23203,7 +23425,7 @@
       </c>
       <c r="CP9">
         <f t="shared" ca="1" si="14"/>
-        <v>0.72949725738773441</v>
+        <v>0.29971412980709966</v>
       </c>
     </row>
     <row r="10" spans="1:97" x14ac:dyDescent="0.35">
@@ -23509,7 +23731,7 @@
       </c>
       <c r="CP10">
         <f t="shared" ca="1" si="14"/>
-        <v>0.78463953172048428</v>
+        <v>0.31900757430696913</v>
       </c>
     </row>
     <row r="11" spans="1:97" x14ac:dyDescent="0.35">
@@ -23816,7 +24038,7 @@
       </c>
       <c r="CP11">
         <f t="shared" ca="1" si="14"/>
-        <v>0.6384152744867877</v>
+        <v>0.111478040888633</v>
       </c>
     </row>
     <row r="12" spans="1:97" x14ac:dyDescent="0.35">
@@ -24122,7 +24344,7 @@
       </c>
       <c r="CP12">
         <f t="shared" ca="1" si="14"/>
-        <v>0.51753202326266357</v>
+        <v>0.23165844663321689</v>
       </c>
     </row>
     <row r="13" spans="1:97" x14ac:dyDescent="0.35">
@@ -24427,7 +24649,7 @@
       </c>
       <c r="CP13">
         <f t="shared" ca="1" si="14"/>
-        <v>0.62944412725725574</v>
+        <v>0.16900600407776656</v>
       </c>
     </row>
     <row r="14" spans="1:97" x14ac:dyDescent="0.35">
@@ -24734,7 +24956,7 @@
       </c>
       <c r="CP14">
         <f t="shared" ca="1" si="14"/>
-        <v>0.58753372320610486</v>
+        <v>5.2120526852199589E-3</v>
       </c>
     </row>
     <row r="15" spans="1:97" x14ac:dyDescent="0.35">
@@ -25041,7 +25263,7 @@
       </c>
       <c r="CP15">
         <f t="shared" ca="1" si="14"/>
-        <v>0.77070614782862545</v>
+        <v>5.6436414968320858E-2</v>
       </c>
     </row>
     <row r="16" spans="1:97" x14ac:dyDescent="0.35">
@@ -25349,7 +25571,7 @@
       </c>
       <c r="CP16">
         <f t="shared" ca="1" si="14"/>
-        <v>2.8998382613760754E-3</v>
+        <v>0.83995417415766183</v>
       </c>
     </row>
     <row r="17" spans="1:94" x14ac:dyDescent="0.35">
@@ -25656,7 +25878,7 @@
       </c>
       <c r="CP17">
         <f t="shared" ca="1" si="14"/>
-        <v>0.77422988281249105</v>
+        <v>0.36312052988540844</v>
       </c>
     </row>
     <row r="18" spans="1:94" x14ac:dyDescent="0.35">
@@ -25962,7 +26184,7 @@
       </c>
       <c r="CP18">
         <f t="shared" ca="1" si="14"/>
-        <v>0.90736734195703717</v>
+        <v>0.44613022748465059</v>
       </c>
     </row>
     <row r="19" spans="1:94" x14ac:dyDescent="0.35">
@@ -26269,7 +26491,7 @@
       </c>
       <c r="CP19">
         <f t="shared" ca="1" si="14"/>
-        <v>0.81217580806472822</v>
+        <v>0.79725105491203596</v>
       </c>
     </row>
     <row r="20" spans="1:94" x14ac:dyDescent="0.35">
@@ -26579,7 +26801,7 @@
       </c>
       <c r="CP20">
         <f t="shared" ca="1" si="14"/>
-        <v>0.94468402641270433</v>
+        <v>0.85170208385498003</v>
       </c>
     </row>
     <row r="21" spans="1:94" x14ac:dyDescent="0.35">
@@ -26887,7 +27109,7 @@
       </c>
       <c r="CP21">
         <f t="shared" ca="1" si="14"/>
-        <v>0.62495145053348777</v>
+        <v>0.78093074054963363</v>
       </c>
     </row>
     <row r="22" spans="1:94" x14ac:dyDescent="0.35">
@@ -27195,7 +27417,7 @@
       </c>
       <c r="CP22">
         <f t="shared" ca="1" si="14"/>
-        <v>0.2392544038465021</v>
+        <v>0.31515346107210584</v>
       </c>
     </row>
     <row r="23" spans="1:94" x14ac:dyDescent="0.35">
@@ -27502,7 +27724,7 @@
       </c>
       <c r="CP23">
         <f t="shared" ca="1" si="14"/>
-        <v>0.83337712393875851</v>
+        <v>0.89395908965128679</v>
       </c>
     </row>
     <row r="24" spans="1:94" x14ac:dyDescent="0.35">
@@ -27810,7 +28032,7 @@
       </c>
       <c r="CP24">
         <f t="shared" ca="1" si="14"/>
-        <v>0.71473446992249678</v>
+        <v>0.66028066377421957</v>
       </c>
     </row>
     <row r="25" spans="1:94" x14ac:dyDescent="0.35">
@@ -28117,7 +28339,7 @@
       </c>
       <c r="CP25">
         <f t="shared" ca="1" si="14"/>
-        <v>0.65450979430393985</v>
+        <v>0.77358150159783323</v>
       </c>
     </row>
     <row r="26" spans="1:94" x14ac:dyDescent="0.35">
@@ -28425,7 +28647,7 @@
       </c>
       <c r="CP26">
         <f t="shared" ca="1" si="14"/>
-        <v>0.9805463939199659</v>
+        <v>0.83647823918299302</v>
       </c>
     </row>
     <row r="27" spans="1:94" x14ac:dyDescent="0.35">
@@ -28733,7 +28955,7 @@
       </c>
       <c r="CP27">
         <f t="shared" ca="1" si="14"/>
-        <v>0.95389613168063414</v>
+        <v>0.65363649645854471</v>
       </c>
     </row>
     <row r="28" spans="1:94" x14ac:dyDescent="0.35">
@@ -29040,7 +29262,7 @@
       </c>
       <c r="CP28">
         <f t="shared" ca="1" si="14"/>
-        <v>0.3486461866562407</v>
+        <v>0.62308942180746485</v>
       </c>
     </row>
     <row r="29" spans="1:94" x14ac:dyDescent="0.35">
@@ -29348,7 +29570,7 @@
       </c>
       <c r="CP29">
         <f t="shared" ca="1" si="14"/>
-        <v>0.56845651663813923</v>
+        <v>0.78789663566133605</v>
       </c>
     </row>
     <row r="30" spans="1:94" x14ac:dyDescent="0.35">
@@ -29657,7 +29879,7 @@
       </c>
       <c r="CP30">
         <f t="shared" ca="1" si="14"/>
-        <v>0.40041112041464688</v>
+        <v>0.67723992541474021</v>
       </c>
     </row>
     <row r="31" spans="1:94" x14ac:dyDescent="0.35">
@@ -29964,7 +30186,7 @@
       </c>
       <c r="CP31">
         <f t="shared" ca="1" si="14"/>
-        <v>0.77809740978952335</v>
+        <v>0.4970477715797722</v>
       </c>
     </row>
     <row r="32" spans="1:94" x14ac:dyDescent="0.35">
@@ -30272,7 +30494,7 @@
       </c>
       <c r="CP32">
         <f t="shared" ca="1" si="14"/>
-        <v>0.27596932357966164</v>
+        <v>0.89520439503975657</v>
       </c>
     </row>
     <row r="33" spans="1:96" x14ac:dyDescent="0.35">
@@ -30577,7 +30799,7 @@
       </c>
       <c r="CP33">
         <f t="shared" ca="1" si="14"/>
-        <v>0.66873102510442339</v>
+        <v>1.4853840821053899E-2</v>
       </c>
       <c r="CR33" s="11"/>
     </row>
@@ -30884,7 +31106,7 @@
       </c>
       <c r="CP34">
         <f t="shared" ca="1" si="14"/>
-        <v>0.50324364883382522</v>
+        <v>0.86657948231528048</v>
       </c>
     </row>
     <row r="35" spans="1:96" x14ac:dyDescent="0.35">
@@ -31195,7 +31417,7 @@
       </c>
       <c r="CP35">
         <f t="shared" ca="1" si="14"/>
-        <v>0.55327226198879287</v>
+        <v>0.74669461346789934</v>
       </c>
     </row>
     <row r="36" spans="1:96" x14ac:dyDescent="0.35">
@@ -31499,7 +31721,7 @@
       </c>
       <c r="CP36">
         <f t="shared" ca="1" si="14"/>
-        <v>0.85672877419051985</v>
+        <v>0.54420325471360653</v>
       </c>
     </row>
     <row r="37" spans="1:96" x14ac:dyDescent="0.35">
@@ -31804,7 +32026,7 @@
       </c>
       <c r="CP37">
         <f t="shared" ca="1" si="14"/>
-        <v>0.32153630140116829</v>
+        <v>0.31389811058993899</v>
       </c>
     </row>
     <row r="38" spans="1:96" x14ac:dyDescent="0.35">
@@ -32109,7 +32331,7 @@
       </c>
       <c r="CP38">
         <f t="shared" ca="1" si="14"/>
-        <v>0.8124277146792086</v>
+        <v>5.956546438335808E-2</v>
       </c>
     </row>
     <row r="39" spans="1:96" x14ac:dyDescent="0.35">
@@ -32415,7 +32637,7 @@
       </c>
       <c r="CP39">
         <f t="shared" ca="1" si="14"/>
-        <v>0.47453720792052234</v>
+        <v>0.29045069381723754</v>
       </c>
     </row>
     <row r="40" spans="1:96" x14ac:dyDescent="0.35">
@@ -32723,7 +32945,7 @@
       </c>
       <c r="CP40">
         <f t="shared" ca="1" si="14"/>
-        <v>0.83876794215654804</v>
+        <v>0.63737052776167213</v>
       </c>
     </row>
     <row r="41" spans="1:96" x14ac:dyDescent="0.35">
@@ -33030,7 +33252,7 @@
       </c>
       <c r="CP41">
         <f t="shared" ca="1" si="14"/>
-        <v>0.38755735051587792</v>
+        <v>0.35208801668260592</v>
       </c>
     </row>
     <row r="42" spans="1:96" x14ac:dyDescent="0.35">
@@ -33337,7 +33559,7 @@
       </c>
       <c r="CP42">
         <f t="shared" ca="1" si="14"/>
-        <v>0.665500996672171</v>
+        <v>0.48889582411648391</v>
       </c>
     </row>
     <row r="43" spans="1:96" x14ac:dyDescent="0.35">
@@ -33645,7 +33867,7 @@
       </c>
       <c r="CP43">
         <f t="shared" ca="1" si="14"/>
-        <v>0.65426078967084933</v>
+        <v>0.61579633964306557</v>
       </c>
     </row>
     <row r="44" spans="1:96" x14ac:dyDescent="0.35">
@@ -33950,7 +34172,7 @@
       </c>
       <c r="CP44">
         <f t="shared" ca="1" si="14"/>
-        <v>0.71212913185135251</v>
+        <v>0.41795499026620386</v>
       </c>
     </row>
     <row r="45" spans="1:96" x14ac:dyDescent="0.35">
@@ -34257,7 +34479,7 @@
       </c>
       <c r="CP45">
         <f t="shared" ca="1" si="14"/>
-        <v>0.48470388647545204</v>
+        <v>0.44120653087900719</v>
       </c>
     </row>
     <row r="46" spans="1:96" x14ac:dyDescent="0.35">
@@ -34565,7 +34787,7 @@
       </c>
       <c r="CP46">
         <f t="shared" ca="1" si="14"/>
-        <v>0.22546805792690994</v>
+        <v>0.36714133777119251</v>
       </c>
     </row>
     <row r="47" spans="1:96" x14ac:dyDescent="0.35">
@@ -34870,7 +35092,7 @@
       </c>
       <c r="CP47">
         <f t="shared" ca="1" si="14"/>
-        <v>0.82355325844510818</v>
+        <v>0.83055195007889959</v>
       </c>
     </row>
     <row r="48" spans="1:96" x14ac:dyDescent="0.35">
@@ -35179,7 +35401,7 @@
       </c>
       <c r="CP48">
         <f t="shared" ca="1" si="14"/>
-        <v>0.92499108265698315</v>
+        <v>0.61902255504282711</v>
       </c>
     </row>
     <row r="49" spans="1:94" x14ac:dyDescent="0.35">
@@ -35486,7 +35708,7 @@
       </c>
       <c r="CP49">
         <f t="shared" ca="1" si="14"/>
-        <v>0.89324463420093814</v>
+        <v>2.871064279294866E-2</v>
       </c>
     </row>
     <row r="50" spans="1:94" x14ac:dyDescent="0.35">
@@ -35793,7 +36015,7 @@
       </c>
       <c r="CP50">
         <f t="shared" ca="1" si="14"/>
-        <v>0.14758094625032425</v>
+        <v>0.16389243015393018</v>
       </c>
     </row>
     <row r="51" spans="1:94" x14ac:dyDescent="0.35">
@@ -36103,7 +36325,7 @@
       </c>
       <c r="CP51">
         <f t="shared" ca="1" si="14"/>
-        <v>0.77430811218196682</v>
+        <v>0.85534594717006163</v>
       </c>
     </row>
     <row r="52" spans="1:94" x14ac:dyDescent="0.35">
@@ -36410,7 +36632,7 @@
       </c>
       <c r="CP52">
         <f t="shared" ca="1" si="14"/>
-        <v>0.6525507912373959</v>
+        <v>0.21958572422135214</v>
       </c>
     </row>
     <row r="53" spans="1:94" x14ac:dyDescent="0.35">
@@ -36715,7 +36937,7 @@
       </c>
       <c r="CP53">
         <f t="shared" ca="1" si="14"/>
-        <v>0.46040829308777786</v>
+        <v>3.650805059429707E-2</v>
       </c>
     </row>
     <row r="54" spans="1:94" x14ac:dyDescent="0.35">
@@ -37022,7 +37244,7 @@
       </c>
       <c r="CP54">
         <f t="shared" ca="1" si="14"/>
-        <v>0.44068932919652037</v>
+        <v>0.51384227593538445</v>
       </c>
     </row>
     <row r="55" spans="1:94" x14ac:dyDescent="0.35">
@@ -37330,7 +37552,7 @@
       </c>
       <c r="CP55">
         <f t="shared" ca="1" si="14"/>
-        <v>0.90404814181011794</v>
+        <v>5.047315819350251E-3</v>
       </c>
     </row>
     <row r="56" spans="1:94" x14ac:dyDescent="0.35">
@@ -37638,7 +37860,7 @@
       </c>
       <c r="CP56">
         <f t="shared" ca="1" si="14"/>
-        <v>0.94017509190955884</v>
+        <v>0.57006923793164599</v>
       </c>
     </row>
     <row r="57" spans="1:94" x14ac:dyDescent="0.35">
@@ -37943,7 +38165,7 @@
       </c>
       <c r="CP57">
         <f t="shared" ca="1" si="14"/>
-        <v>6.4354637126682324E-2</v>
+        <v>0.366915692955888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>